<commit_message>
Updated CHE model - 2025-08-16 18:10
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7079ACE-8EA1-4949-8CC9-956BA62F030F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{398E2FA7-BE01-4237-A61D-02DD81742470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1022" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1026" uniqueCount="247">
   <si>
     <t>~FI_Process</t>
   </si>
@@ -111,9 +111,6 @@
   </si>
   <si>
     <t>elc_buildings,elc_industry,elc_transport</t>
-  </si>
-  <si>
-    <t>elc_demand</t>
   </si>
   <si>
     <t>~FI_Comm</t>
@@ -401,9 +398,6 @@
     <t>Car battery - 6kw/60Kwh - with V2G (optional)</t>
   </si>
   <si>
-    <t>EV_Battery</t>
-  </si>
-  <si>
     <t>elc_roadtransport</t>
   </si>
   <si>
@@ -428,6 +422,21 @@
     <t>~FI_T: USD21~FX~ACT_BND</t>
   </si>
   <si>
+    <t>ev_battery</t>
+  </si>
+  <si>
+    <t>e_demand</t>
+  </si>
+  <si>
+    <t>life</t>
+  </si>
+  <si>
+    <t>Demand sectors</t>
+  </si>
+  <si>
+    <t>generic fuel supply</t>
+  </si>
+  <si>
     <t>~fi_process</t>
   </si>
   <si>
@@ -491,24 +500,24 @@
     <t>ele</t>
   </si>
   <si>
+    <t>e_spv-CHE_15_c3</t>
+  </si>
+  <si>
+    <t>solar resource -- CF class spv-CHE_15 -- cost class 3</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
     <t>e_spv-CHE_15_c2</t>
   </si>
   <si>
     <t>solar resource -- CF class spv-CHE_15 -- cost class 2</t>
   </si>
   <si>
-    <t>annual</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>e_spv-CHE_15_c3</t>
-  </si>
-  <si>
-    <t>solar resource -- CF class spv-CHE_15 -- cost class 3</t>
-  </si>
-  <si>
     <t>e_spv-CHE_15_c1</t>
   </si>
   <si>
@@ -659,18 +668,18 @@
     <t>wind resource -- CF class won-CHE_22 -- cost class 3</t>
   </si>
   <si>
+    <t>e_won-CHE_20_c2</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-CHE_20 -- cost class 2</t>
+  </si>
+  <si>
     <t>e_won-CHE_20_c1</t>
   </si>
   <si>
     <t>wind resource -- CF class won-CHE_20 -- cost class 1</t>
   </si>
   <si>
-    <t>e_won-CHE_20_c2</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-CHE_20 -- cost class 2</t>
-  </si>
-  <si>
     <t>e_won-CHE_18_c2</t>
   </si>
   <si>
@@ -713,16 +722,16 @@
     <t>wind resource -- CF class won-CHE_16 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-CHE_16_c2</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-CHE_16 -- cost class 2</t>
+  </si>
+  <si>
     <t>e_won-CHE_16_c3</t>
   </si>
   <si>
     <t>wind resource -- CF class won-CHE_16 -- cost class 3</t>
-  </si>
-  <si>
-    <t>e_won-CHE_16_c2</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-CHE_16 -- cost class 2</t>
   </si>
   <si>
     <t>e_won-CHE_15_c1</t>
@@ -1212,7 +1221,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{54EAAA90-32CC-6ECA-C3B5-F7197FA49364}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F57F225B-449B-0A31-AAEF-5355EEE29B47}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1267,7 +1276,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F9D88427-7C84-8BC4-F28C-612F0FC304AC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6998E14A-D71B-790A-D7D3-7B3AFAE2D8E6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1322,7 +1331,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5F99329C-EB3D-57FD-3FA1-281E78A8AECA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44B01E60-5C1C-919C-C440-D6926EAC786E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1377,7 +1386,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EF7D4CF-59DA-A28A-0251-C3B1C7EAA930}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E34A19BF-D748-BCD1-BF0F-423BD8E750FC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1675,10 +1684,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{034C1C47-C7B1-48B4-9602-2B825216B37E}">
-  <dimension ref="B2:T18"/>
+  <dimension ref="B2:V18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1698,19 +1707,19 @@
     <col min="17" max="17" width="3.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:20" ht="14.65" thickBot="1">
+    <row r="2" spans="2:22" ht="14.65" thickBot="1">
       <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
       <c r="Q2" s="1"/>
     </row>
-    <row r="3" spans="2:20">
+    <row r="3" spans="2:22">
       <c r="B3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1745,7 +1754,7 @@
         <v>5</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P3" s="1">
         <v>2022</v>
@@ -1753,8 +1762,14 @@
       <c r="Q3" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="2:20">
+      <c r="R3" t="s">
+        <v>103</v>
+      </c>
+      <c r="S3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="2:22">
       <c r="B4" s="1" t="s">
         <v>17</v>
       </c>
@@ -1787,7 +1802,7 @@
       <c r="P4" s="1"/>
       <c r="Q4" s="1"/>
     </row>
-    <row r="5" spans="2:20">
+    <row r="5" spans="2:22">
       <c r="B5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1822,14 +1837,16 @@
       <c r="P5" s="1"/>
       <c r="Q5" s="1"/>
     </row>
-    <row r="6" spans="2:20">
+    <row r="6" spans="2:22">
       <c r="B6" t="s">
         <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6" s="1"/>
+        <v>106</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>108</v>
+      </c>
       <c r="E6" s="1" t="s">
         <v>21</v>
       </c>
@@ -1841,7 +1858,7 @@
       <c r="I6" s="1"/>
       <c r="J6" s="1" t="str">
         <f>C6</f>
-        <v>elc_demand</v>
+        <v>e_demand</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>19</v>
@@ -1858,18 +1875,20 @@
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
       <c r="Q6" s="1"/>
-      <c r="T6" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="7" spans="2:20">
+      <c r="V6" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="7" spans="2:22">
       <c r="B7" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>109</v>
+      </c>
       <c r="E7" s="1" t="s">
         <v>21</v>
       </c>
@@ -1885,25 +1904,25 @@
       </c>
       <c r="K7" s="1"/>
       <c r="L7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1">
-        <f t="shared" ref="O7:O16" si="0">T7*3.6</f>
+        <f t="shared" ref="O7:O16" si="0">V7*3.6</f>
         <v>25.2</v>
       </c>
       <c r="P7" s="1"/>
-      <c r="T7" s="1">
+      <c r="V7" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="2:20">
+    <row r="8" spans="2:22">
       <c r="B8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
@@ -1917,7 +1936,7 @@
       <c r="I8" s="1"/>
       <c r="K8" s="1"/>
       <c r="L8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
@@ -1926,16 +1945,16 @@
         <v>7.2</v>
       </c>
       <c r="P8" s="1"/>
-      <c r="T8" s="1">
+      <c r="V8" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="2:20">
+    <row r="9" spans="2:22">
       <c r="B9" t="s">
+        <v>99</v>
+      </c>
+      <c r="C9" t="s">
         <v>101</v>
-      </c>
-      <c r="C9" t="s">
-        <v>103</v>
       </c>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
@@ -1949,7 +1968,7 @@
       <c r="I9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -1958,11 +1977,11 @@
         <v>18</v>
       </c>
       <c r="P9" s="1"/>
-      <c r="T9" s="1">
+      <c r="V9" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:20">
+    <row r="10" spans="2:22">
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
@@ -1974,7 +1993,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -1983,11 +2002,11 @@
         <v>0.36000000000000004</v>
       </c>
       <c r="P10" s="1"/>
-      <c r="T10">
+      <c r="V10">
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="2:20">
+    <row r="11" spans="2:22">
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
@@ -1999,7 +2018,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
       <c r="L11" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
@@ -2008,11 +2027,11 @@
         <v>0.36000000000000004</v>
       </c>
       <c r="P11" s="1"/>
-      <c r="T11">
+      <c r="V11">
         <v>0.1</v>
       </c>
     </row>
-    <row r="12" spans="2:20">
+    <row r="12" spans="2:22">
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
@@ -2024,7 +2043,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
@@ -2033,11 +2052,11 @@
         <v>108</v>
       </c>
       <c r="P12" s="1"/>
-      <c r="T12">
+      <c r="V12">
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="2:20">
+    <row r="13" spans="2:22">
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -2049,7 +2068,7 @@
       <c r="J13" s="1"/>
       <c r="K13" s="1"/>
       <c r="L13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
@@ -2058,11 +2077,11 @@
         <v>0.36000000000000004</v>
       </c>
       <c r="P13" s="1"/>
-      <c r="T13">
+      <c r="V13">
         <v>0.1</v>
       </c>
     </row>
-    <row r="14" spans="2:20">
+    <row r="14" spans="2:22">
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -2074,7 +2093,7 @@
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
@@ -2083,11 +2102,11 @@
         <v>36</v>
       </c>
       <c r="P14" s="1"/>
-      <c r="T14">
+      <c r="V14">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:20">
+    <row r="15" spans="2:22">
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
@@ -2099,7 +2118,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
       <c r="L15" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
@@ -2108,11 +2127,11 @@
         <v>0.36000000000000004</v>
       </c>
       <c r="P15" s="1"/>
-      <c r="T15">
+      <c r="V15">
         <v>0.1</v>
       </c>
     </row>
-    <row r="16" spans="2:20">
+    <row r="16" spans="2:22">
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
@@ -2124,7 +2143,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
@@ -2133,11 +2152,11 @@
         <v>0.36000000000000004</v>
       </c>
       <c r="P16" s="1"/>
-      <c r="T16">
+      <c r="V16">
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="10:17">
+    <row r="17" spans="10:19">
       <c r="J17" t="str">
         <f>C8</f>
         <v>Trd_electricity import</v>
@@ -2151,8 +2170,14 @@
       <c r="Q17">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="10:17">
+      <c r="R17">
+        <v>1000</v>
+      </c>
+      <c r="S17">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="10:19">
       <c r="J18" t="str">
         <f>C9</f>
         <v>Trd_electricity export</v>
@@ -2165,6 +2190,12 @@
       </c>
       <c r="Q18">
         <v>3</v>
+      </c>
+      <c r="R18">
+        <v>1000</v>
+      </c>
+      <c r="S18">
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2197,7 +2228,7 @@
   <sheetData>
     <row r="1" spans="1:14" ht="22.05" customHeight="1">
       <c r="A1" s="27" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -2209,10 +2240,10 @@
     </row>
     <row r="2" spans="1:14" ht="14.65" thickBot="1">
       <c r="B2" s="28" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="I2" s="28" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="15.75" thickBot="1">
@@ -2220,10 +2251,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E3" s="29" t="s">
         <v>9</v>
@@ -2232,10 +2263,10 @@
         <v>8</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="I3" s="29" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="J3" s="29" t="s">
         <v>2</v>
@@ -2244,13 +2275,13 @@
         <v>3</v>
       </c>
       <c r="L3" s="29" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="M3" s="29" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="N3" s="29" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -2258,13 +2289,13 @@
         <v>17</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="E4" s="30" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F4" s="30" t="s">
         <v>10</v>
@@ -2273,10 +2304,10 @@
         <v>14</v>
       </c>
       <c r="I4" s="30" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="J4" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K4" s="30" t="s">
         <v>19</v>
@@ -2292,13 +2323,13 @@
         <v>17</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="E5" s="31" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F5" s="31" t="s">
         <v>10</v>
@@ -2307,10 +2338,10 @@
         <v>14</v>
       </c>
       <c r="I5" s="31" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="J5" s="31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K5" s="31" t="s">
         <v>19</v>
@@ -2326,13 +2357,13 @@
         <v>17</v>
       </c>
       <c r="C6" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="E6" s="30" t="s">
         <v>116</v>
-      </c>
-      <c r="D6" s="30" t="s">
-        <v>117</v>
-      </c>
-      <c r="E6" s="30" t="s">
-        <v>113</v>
       </c>
       <c r="F6" s="30" t="s">
         <v>10</v>
@@ -2341,10 +2372,10 @@
         <v>14</v>
       </c>
       <c r="I6" s="30" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="J6" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="K6" s="30" t="s">
         <v>19</v>
@@ -2368,7 +2399,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7FD6D8AA-F8A9-4BBE-94C7-C767CA3BCC03}">
   <dimension ref="B2:W61"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25"/>
   <cols>
@@ -2396,7 +2429,7 @@
   <sheetData>
     <row r="2" spans="2:23">
       <c r="B2" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -2408,42 +2441,42 @@
     </row>
     <row r="3" spans="2:23">
       <c r="B3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="G3" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="4" spans="2:23">
       <c r="B4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>51</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="5" t="s">
@@ -2454,13 +2487,13 @@
     </row>
     <row r="5" spans="2:23">
       <c r="C5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="E5" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="5" t="s">
@@ -2482,7 +2515,7 @@
       <c r="K8" s="6"/>
       <c r="L8" s="6"/>
       <c r="M8" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="O8" s="6"/>
       <c r="P8" s="6"/>
@@ -2505,10 +2538,10 @@
         <v>7</v>
       </c>
       <c r="E9" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="F9" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="F9" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>11</v>
@@ -2518,16 +2551,16 @@
         <v>1</v>
       </c>
       <c r="J9" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="K9" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="K9" s="6" t="s">
+      <c r="L9" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M9" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="L9" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="M9" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="N9" s="6">
         <f>J35</f>
@@ -2561,24 +2594,24 @@
         <v>3</v>
       </c>
       <c r="V9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="W9" t="s">
         <v>60</v>
-      </c>
-      <c r="W9" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" spans="2:23">
       <c r="B10" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="D10" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="8" t="s">
-        <v>64</v>
-      </c>
       <c r="E10" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F10" s="5" t="s">
         <v>10</v>
@@ -2588,13 +2621,13 @@
       </c>
       <c r="H10" s="6"/>
       <c r="I10" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="J10" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="J10" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="K10" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L10" s="3" t="s">
         <v>19</v>
@@ -2624,13 +2657,13 @@
     <row r="11" spans="2:23">
       <c r="B11" s="5"/>
       <c r="C11" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D11" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F11" s="5" t="s">
         <v>10</v>
@@ -2640,13 +2673,13 @@
       </c>
       <c r="H11" s="6"/>
       <c r="I11" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J11" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="K11" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="K11" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="L11" s="6" t="s">
         <v>19</v>
@@ -2678,13 +2711,13 @@
       <c r="G12" s="5"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J12" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K12" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L12" s="6"/>
       <c r="M12" s="7" t="s">
@@ -2711,10 +2744,10 @@
       <c r="G13" s="5"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J13" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K13" s="6"/>
       <c r="L13" s="6"/>
@@ -2752,10 +2785,10 @@
     </row>
     <row r="14" spans="2:23">
       <c r="I14" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N14" s="4">
         <f>J44</f>
@@ -2788,10 +2821,10 @@
     </row>
     <row r="15" spans="2:23">
       <c r="I15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M15" t="s">
         <v>18</v>
@@ -2808,10 +2841,10 @@
     </row>
     <row r="16" spans="2:23">
       <c r="I16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J16" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N16" s="9">
         <v>31.536000000000001</v>
@@ -2825,10 +2858,10 @@
     </row>
     <row r="17" spans="9:23">
       <c r="I17" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="J17" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N17" s="4">
         <v>0.85</v>
@@ -2842,13 +2875,13 @@
     </row>
     <row r="18" spans="9:23">
       <c r="I18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L18" s="3" t="s">
         <v>19</v>
@@ -2877,13 +2910,13 @@
     </row>
     <row r="19" spans="9:23">
       <c r="I19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J19" t="s">
+        <v>67</v>
+      </c>
+      <c r="K19" t="s">
         <v>68</v>
-      </c>
-      <c r="K19" t="s">
-        <v>69</v>
       </c>
       <c r="L19" t="s">
         <v>19</v>
@@ -2908,13 +2941,13 @@
     </row>
     <row r="20" spans="9:23">
       <c r="I20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J20" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="K20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="M20" t="s">
         <v>14</v>
@@ -2931,10 +2964,10 @@
     </row>
     <row r="21" spans="9:23">
       <c r="I21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="N21" s="4">
         <f>J49</f>
@@ -2967,10 +3000,10 @@
     </row>
     <row r="22" spans="9:23">
       <c r="I22" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="N22" s="4">
         <f>J53</f>
@@ -3003,10 +3036,10 @@
     </row>
     <row r="23" spans="9:23">
       <c r="I23" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M23" t="s">
         <v>18</v>
@@ -3023,10 +3056,10 @@
     </row>
     <row r="24" spans="9:23">
       <c r="I24" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J24" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="N24" s="9">
         <v>31.536000000000001</v>
@@ -3040,10 +3073,10 @@
     </row>
     <row r="25" spans="9:23">
       <c r="I25" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J25" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="N25" s="4">
         <v>0.85</v>
@@ -3057,7 +3090,7 @@
     </row>
     <row r="31" spans="9:23" ht="15.75">
       <c r="I31" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J31" s="11"/>
       <c r="K31" s="11"/>
@@ -3069,7 +3102,7 @@
     </row>
     <row r="32" spans="9:23" ht="15.75">
       <c r="I32" s="10" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J32" s="11"/>
       <c r="K32" s="11"/>
@@ -3091,7 +3124,7 @@
     </row>
     <row r="34" spans="9:16" ht="15.75">
       <c r="I34" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="J34" s="14"/>
       <c r="K34" s="14"/>
@@ -3127,7 +3160,7 @@
     </row>
     <row r="36" spans="9:16" ht="15.75">
       <c r="I36" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="J36" s="14"/>
       <c r="K36" s="14"/>
@@ -3139,7 +3172,7 @@
     </row>
     <row r="37" spans="9:16" ht="15.75">
       <c r="I37" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J37" s="14"/>
       <c r="K37" s="14"/>
@@ -3151,7 +3184,7 @@
     </row>
     <row r="38" spans="9:16" ht="15.75">
       <c r="I38" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J38" s="16">
         <v>1363</v>
@@ -3177,7 +3210,7 @@
     </row>
     <row r="39" spans="9:16" ht="15.75">
       <c r="I39" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J39" s="16">
         <v>1363</v>
@@ -3203,7 +3236,7 @@
     </row>
     <row r="40" spans="9:16" ht="15.75">
       <c r="I40" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J40" s="16">
         <v>1363</v>
@@ -3229,7 +3262,7 @@
     </row>
     <row r="41" spans="9:16" ht="15.75">
       <c r="I41" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J41" s="17"/>
       <c r="K41" s="17"/>
@@ -3241,7 +3274,7 @@
     </row>
     <row r="42" spans="9:16" ht="15.75">
       <c r="I42" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J42" s="18">
         <v>34</v>
@@ -3267,7 +3300,7 @@
     </row>
     <row r="43" spans="9:16" ht="15.75">
       <c r="I43" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J43" s="18">
         <v>34</v>
@@ -3293,7 +3326,7 @@
     </row>
     <row r="44" spans="9:16" ht="15.75">
       <c r="I44" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J44" s="18">
         <v>34</v>
@@ -3319,7 +3352,7 @@
     </row>
     <row r="45" spans="9:16" ht="15.75">
       <c r="I45" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J45" s="17"/>
       <c r="K45" s="17"/>
@@ -3331,7 +3364,7 @@
     </row>
     <row r="46" spans="9:16" ht="15.75">
       <c r="I46" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="J46" s="17"/>
       <c r="K46" s="17"/>
@@ -3343,7 +3376,7 @@
     </row>
     <row r="47" spans="9:16" ht="15.75">
       <c r="I47" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J47" s="16">
         <v>2470</v>
@@ -3369,7 +3402,7 @@
     </row>
     <row r="48" spans="9:16" ht="15.75">
       <c r="I48" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J48" s="16">
         <v>2470</v>
@@ -3395,7 +3428,7 @@
     </row>
     <row r="49" spans="9:16" ht="15.75">
       <c r="I49" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J49" s="16">
         <v>2470</v>
@@ -3421,7 +3454,7 @@
     </row>
     <row r="50" spans="9:16" ht="15.75">
       <c r="I50" s="13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J50" s="17"/>
       <c r="K50" s="17"/>
@@ -3433,7 +3466,7 @@
     </row>
     <row r="51" spans="9:16" ht="15.75">
       <c r="I51" s="14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J51" s="18">
         <v>62</v>
@@ -3459,7 +3492,7 @@
     </row>
     <row r="52" spans="9:16" ht="15.75">
       <c r="I52" s="14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J52" s="18">
         <v>62</v>
@@ -3485,7 +3518,7 @@
     </row>
     <row r="53" spans="9:16" ht="15.75">
       <c r="I53" s="14" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J53" s="18">
         <v>62</v>
@@ -3521,7 +3554,7 @@
     </row>
     <row r="55" spans="9:16" ht="15.75">
       <c r="I55" s="11" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J55" s="11">
         <v>0.85</v>
@@ -3535,7 +3568,7 @@
     </row>
     <row r="56" spans="9:16" ht="15.75">
       <c r="I56" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="J56" s="11"/>
       <c r="K56" s="11"/>
@@ -3547,7 +3580,7 @@
     </row>
     <row r="57" spans="9:16" ht="15.75">
       <c r="I57" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="J57" s="11"/>
       <c r="K57" s="11"/>
@@ -3608,7 +3641,7 @@
   <dimension ref="B3:Y8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N6" sqref="N6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -3645,7 +3678,7 @@
       <c r="F3" s="23"/>
       <c r="G3" s="23"/>
       <c r="H3" s="23" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I3" s="23"/>
       <c r="J3" s="23"/>
@@ -3678,16 +3711,16 @@
         <v>3</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" t="s">
         <v>89</v>
-      </c>
-      <c r="H4" t="s">
-        <v>90</v>
       </c>
       <c r="I4">
         <v>2030</v>
@@ -3696,22 +3729,22 @@
         <v>0</v>
       </c>
       <c r="K4" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="L4" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="L4" s="23" t="s">
+      <c r="M4" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="N4" s="23" t="s">
+        <v>103</v>
+      </c>
+      <c r="O4" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="M4" s="23" t="s">
-        <v>61</v>
-      </c>
-      <c r="N4" s="23" t="s">
-        <v>105</v>
-      </c>
-      <c r="O4" s="23" t="s">
+      <c r="P4" s="23" t="s">
         <v>93</v>
-      </c>
-      <c r="P4" s="23" t="s">
-        <v>94</v>
       </c>
       <c r="Q4" s="23"/>
       <c r="R4" s="23" t="s">
@@ -3724,30 +3757,30 @@
         <v>7</v>
       </c>
       <c r="U4" s="23" t="s">
+        <v>54</v>
+      </c>
+      <c r="V4" s="23" t="s">
         <v>55</v>
-      </c>
-      <c r="V4" s="23" t="s">
-        <v>56</v>
       </c>
       <c r="W4" s="23" t="s">
         <v>11</v>
       </c>
       <c r="X4" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y4" s="23" t="s">
         <v>95</v>
       </c>
-      <c r="Y4" s="23" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="5" spans="2:25">
-      <c r="B5" s="23" t="s">
-        <v>98</v>
+      <c r="B5" t="s">
+        <v>105</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="F5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K5" s="23">
         <v>0.90249999999999997</v>
@@ -3770,14 +3803,14 @@
       </c>
       <c r="Q5" s="23"/>
       <c r="R5" s="23" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="S5" s="23" t="str">
         <f>B5</f>
-        <v>EV_Battery</v>
+        <v>ev_battery</v>
       </c>
       <c r="T5" s="23" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="U5" s="23" t="s">
         <v>21</v>
@@ -3794,7 +3827,7 @@
     <row r="6" spans="2:25">
       <c r="B6" s="23"/>
       <c r="F6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="K6" s="23"/>
       <c r="L6" s="24">
@@ -3817,10 +3850,10 @@
     <row r="7" spans="2:25">
       <c r="B7" s="23"/>
       <c r="D7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="K7" s="23"/>
       <c r="L7" s="23"/>
@@ -3850,7 +3883,7 @@
         <v>AuxStoIN</v>
       </c>
       <c r="H8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I8">
         <v>1</v>
@@ -3880,7 +3913,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42A4F212-722B-437A-9D02-C0AA30C98C6B}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4186DA58-E7A0-4982-96AF-F2941C12B474}">
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3904,7 +3937,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="22.05" customHeight="1">
       <c r="A1" s="27" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -3916,62 +3949,62 @@
     </row>
     <row r="2" spans="1:16" ht="14.65" thickBot="1">
       <c r="B2" s="28" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="K2" s="28" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1">
       <c r="B3" s="29" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="L3" s="29" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="M3" s="29" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="N3" s="29" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="O3" s="29" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="P3" s="29" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="B4" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="E4" s="30" t="s">
         <v>10</v>
@@ -3980,39 +4013,39 @@
         <v>21</v>
       </c>
       <c r="G4" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H4" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="K4" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="K4" s="30" t="s">
-        <v>128</v>
-      </c>
       <c r="L4" s="30" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="M4" s="34">
-        <v>4.725E-2</v>
+        <v>6.7499999999999999E-3</v>
       </c>
       <c r="N4" s="34">
         <v>0.14799999999999999</v>
       </c>
       <c r="O4" s="32">
-        <v>57.399715057025539</v>
+        <v>58.670132479893049</v>
       </c>
       <c r="P4" s="35">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="B5" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="E5" s="31" t="s">
         <v>10</v>
@@ -4021,39 +4054,39 @@
         <v>21</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K5" s="31" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="L5" s="31" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="M5" s="36">
-        <v>6.7499999999999999E-3</v>
+        <v>4.725E-2</v>
       </c>
       <c r="N5" s="36">
         <v>0.14799999999999999</v>
       </c>
       <c r="O5" s="33">
-        <v>58.670132479893049</v>
+        <v>57.399715057025539</v>
       </c>
       <c r="P5" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="B6" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="E6" s="30" t="s">
         <v>10</v>
@@ -4062,16 +4095,16 @@
         <v>21</v>
       </c>
       <c r="G6" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K6" s="30" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="L6" s="30" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="M6" s="34">
         <v>0.44700000000000001</v>
@@ -4088,13 +4121,13 @@
     </row>
     <row r="7" spans="1:16">
       <c r="B7" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="E7" s="31" t="s">
         <v>10</v>
@@ -4103,16 +4136,16 @@
         <v>21</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K7" s="31" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="L7" s="31" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="M7" s="36">
         <v>0.15075</v>
@@ -4129,13 +4162,13 @@
     </row>
     <row r="8" spans="1:16">
       <c r="B8" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="E8" s="30" t="s">
         <v>10</v>
@@ -4144,16 +4177,16 @@
         <v>21</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K8" s="30" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="L8" s="30" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="M8" s="34">
         <v>0.60075000000000001</v>
@@ -4170,13 +4203,13 @@
     </row>
     <row r="9" spans="1:16">
       <c r="B9" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="E9" s="31" t="s">
         <v>10</v>
@@ -4185,16 +4218,16 @@
         <v>21</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H9" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K9" s="31" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="L9" s="31" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="M9" s="36">
         <v>2.3692500000000001</v>
@@ -4211,13 +4244,13 @@
     </row>
     <row r="10" spans="1:16">
       <c r="B10" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="E10" s="30" t="s">
         <v>10</v>
@@ -4226,16 +4259,16 @@
         <v>21</v>
       </c>
       <c r="G10" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K10" s="30" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="L10" s="30" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="M10" s="34">
         <v>2.7854999999999999</v>
@@ -4252,13 +4285,13 @@
     </row>
     <row r="11" spans="1:16">
       <c r="B11" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="E11" s="31" t="s">
         <v>10</v>
@@ -4267,16 +4300,16 @@
         <v>21</v>
       </c>
       <c r="G11" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K11" s="31" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="M11" s="36">
         <v>3.6675</v>
@@ -4293,13 +4326,13 @@
     </row>
     <row r="12" spans="1:16">
       <c r="B12" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="E12" s="30" t="s">
         <v>10</v>
@@ -4308,16 +4341,16 @@
         <v>21</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K12" s="30" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="L12" s="30" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="M12" s="34">
         <v>6.1710000000000003</v>
@@ -4334,13 +4367,13 @@
     </row>
     <row r="13" spans="1:16">
       <c r="B13" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>10</v>
@@ -4349,16 +4382,16 @@
         <v>21</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K13" s="31" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="L13" s="31" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="M13" s="36">
         <v>7.2007500000000002</v>
@@ -4375,13 +4408,13 @@
     </row>
     <row r="14" spans="1:16">
       <c r="B14" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="E14" s="30" t="s">
         <v>10</v>
@@ -4390,16 +4423,16 @@
         <v>21</v>
       </c>
       <c r="G14" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H14" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K14" s="30" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="L14" s="30" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="M14" s="34">
         <v>5.1719999999999997</v>
@@ -4416,13 +4449,13 @@
     </row>
     <row r="15" spans="1:16">
       <c r="B15" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>10</v>
@@ -4431,16 +4464,16 @@
         <v>21</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H15" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K15" s="31" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="L15" s="31" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="M15" s="36">
         <v>8.8019999999999996</v>
@@ -4457,13 +4490,13 @@
     </row>
     <row r="16" spans="1:16">
       <c r="B16" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="E16" s="30" t="s">
         <v>10</v>
@@ -4472,16 +4505,16 @@
         <v>21</v>
       </c>
       <c r="G16" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H16" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K16" s="30" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="L16" s="30" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="M16" s="34">
         <v>5.5365000000000002</v>
@@ -4498,13 +4531,13 @@
     </row>
     <row r="17" spans="2:16">
       <c r="B17" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E17" s="31" t="s">
         <v>10</v>
@@ -4513,16 +4546,16 @@
         <v>21</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H17" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K17" s="31" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="L17" s="31" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="M17" s="36">
         <v>2.2499999999999998E-3</v>
@@ -4539,13 +4572,13 @@
     </row>
     <row r="18" spans="2:16">
       <c r="B18" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="E18" s="30" t="s">
         <v>10</v>
@@ -4554,16 +4587,16 @@
         <v>21</v>
       </c>
       <c r="G18" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H18" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K18" s="30" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="L18" s="30" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="M18" s="34">
         <v>8.2500000000000004E-3</v>
@@ -4588,7 +4621,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29440072-DE5D-4796-9252-DB3F9EA50313}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E354DA90-C15C-4AB0-B806-99F5508204B4}">
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4612,7 +4645,7 @@
   <sheetData>
     <row r="1" spans="1:16" ht="22.05" customHeight="1">
       <c r="A1" s="27" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -4624,62 +4657,62 @@
     </row>
     <row r="2" spans="1:16" ht="14.65" thickBot="1">
       <c r="B2" s="28" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="K2" s="28" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" thickBot="1">
       <c r="B3" s="29" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="E3" s="29" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="F3" s="29" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="G3" s="29" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="L3" s="29" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="M3" s="29" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="N3" s="29" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="O3" s="29" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="P3" s="29" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="B4" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="D4" s="30" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="E4" s="30" t="s">
         <v>10</v>
@@ -4688,16 +4721,16 @@
         <v>21</v>
       </c>
       <c r="G4" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K4" s="30" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="L4" s="30" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M4" s="35">
         <v>0.44850000000000001</v>
@@ -4714,13 +4747,13 @@
     </row>
     <row r="5" spans="1:16">
       <c r="B5" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="E5" s="31" t="s">
         <v>10</v>
@@ -4729,16 +4762,16 @@
         <v>21</v>
       </c>
       <c r="G5" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K5" s="31" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="L5" s="31" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M5" s="37">
         <v>7.5884999999999998</v>
@@ -4755,13 +4788,13 @@
     </row>
     <row r="6" spans="1:16">
       <c r="B6" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="D6" s="30" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="E6" s="30" t="s">
         <v>10</v>
@@ -4770,16 +4803,16 @@
         <v>21</v>
       </c>
       <c r="G6" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K6" s="30" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="L6" s="30" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M6" s="35">
         <v>0.90225</v>
@@ -4796,13 +4829,13 @@
     </row>
     <row r="7" spans="1:16">
       <c r="B7" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="D7" s="31" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="E7" s="31" t="s">
         <v>10</v>
@@ -4811,16 +4844,16 @@
         <v>21</v>
       </c>
       <c r="G7" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K7" s="31" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="L7" s="31" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M7" s="37">
         <v>0.85575000000000001</v>
@@ -4837,13 +4870,13 @@
     </row>
     <row r="8" spans="1:16">
       <c r="B8" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="D8" s="30" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="E8" s="30" t="s">
         <v>10</v>
@@ -4852,16 +4885,16 @@
         <v>21</v>
       </c>
       <c r="G8" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K8" s="30" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="L8" s="30" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M8" s="35">
         <v>0.71025000000000005</v>
@@ -4878,13 +4911,13 @@
     </row>
     <row r="9" spans="1:16">
       <c r="B9" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="E9" s="31" t="s">
         <v>10</v>
@@ -4893,16 +4926,16 @@
         <v>21</v>
       </c>
       <c r="G9" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H9" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K9" s="31" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="L9" s="31" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M9" s="37">
         <v>7.6980000000000004</v>
@@ -4919,13 +4952,13 @@
     </row>
     <row r="10" spans="1:16">
       <c r="B10" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="D10" s="30" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="E10" s="30" t="s">
         <v>10</v>
@@ -4934,16 +4967,16 @@
         <v>21</v>
       </c>
       <c r="G10" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K10" s="30" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="L10" s="30" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M10" s="35">
         <v>0.46800000000000003</v>
@@ -4960,13 +4993,13 @@
     </row>
     <row r="11" spans="1:16">
       <c r="B11" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="E11" s="31" t="s">
         <v>10</v>
@@ -4975,16 +5008,16 @@
         <v>21</v>
       </c>
       <c r="G11" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K11" s="31" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M11" s="37">
         <v>7.4332500000000001</v>
@@ -5001,13 +5034,13 @@
     </row>
     <row r="12" spans="1:16">
       <c r="B12" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="D12" s="30" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E12" s="30" t="s">
         <v>10</v>
@@ -5016,16 +5049,16 @@
         <v>21</v>
       </c>
       <c r="G12" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K12" s="30" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="L12" s="30" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M12" s="35">
         <v>6.7035</v>
@@ -5042,13 +5075,13 @@
     </row>
     <row r="13" spans="1:16">
       <c r="B13" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E13" s="31" t="s">
         <v>10</v>
@@ -5057,39 +5090,39 @@
         <v>21</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K13" s="31" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="L13" s="31" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M13" s="37">
-        <v>4.6582499999999998</v>
+        <v>0.30525000000000002</v>
       </c>
       <c r="N13" s="36">
         <v>0.19600000000000001</v>
       </c>
       <c r="O13" s="33">
-        <v>91.771393190446332</v>
+        <v>170.53727340823224</v>
       </c>
       <c r="P13" s="37">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="B14" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="D14" s="30" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="E14" s="30" t="s">
         <v>10</v>
@@ -5098,39 +5131,39 @@
         <v>21</v>
       </c>
       <c r="G14" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H14" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K14" s="30" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="L14" s="30" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M14" s="35">
-        <v>0.30525000000000002</v>
+        <v>4.6582499999999998</v>
       </c>
       <c r="N14" s="34">
         <v>0.19600000000000001</v>
       </c>
       <c r="O14" s="32">
-        <v>170.53727340823224</v>
+        <v>91.771393190446332</v>
       </c>
       <c r="P14" s="35">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="B15" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="E15" s="31" t="s">
         <v>10</v>
@@ -5139,16 +5172,16 @@
         <v>21</v>
       </c>
       <c r="G15" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H15" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K15" s="31" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="L15" s="31" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M15" s="37">
         <v>0.35399999999999998</v>
@@ -5165,13 +5198,13 @@
     </row>
     <row r="16" spans="1:16">
       <c r="B16" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="D16" s="30" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="E16" s="30" t="s">
         <v>10</v>
@@ -5180,16 +5213,16 @@
         <v>21</v>
       </c>
       <c r="G16" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H16" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K16" s="30" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="L16" s="30" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M16" s="35">
         <v>6.3525</v>
@@ -5206,13 +5239,13 @@
     </row>
     <row r="17" spans="2:16">
       <c r="B17" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="E17" s="31" t="s">
         <v>10</v>
@@ -5221,16 +5254,16 @@
         <v>21</v>
       </c>
       <c r="G17" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H17" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K17" s="31" t="s">
-        <v>192</v>
+        <v>195</v>
       </c>
       <c r="L17" s="31" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M17" s="37">
         <v>1.0920000000000001</v>
@@ -5247,13 +5280,13 @@
     </row>
     <row r="18" spans="2:16">
       <c r="B18" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="E18" s="30" t="s">
         <v>10</v>
@@ -5262,16 +5295,16 @@
         <v>21</v>
       </c>
       <c r="G18" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H18" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K18" s="30" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="L18" s="30" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M18" s="35">
         <v>0.55874999999999997</v>
@@ -5288,13 +5321,13 @@
     </row>
     <row r="19" spans="2:16">
       <c r="B19" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="E19" s="31" t="s">
         <v>10</v>
@@ -5303,16 +5336,16 @@
         <v>21</v>
       </c>
       <c r="G19" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H19" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K19" s="31" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="L19" s="31" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M19" s="37">
         <v>7.33575</v>
@@ -5329,13 +5362,13 @@
     </row>
     <row r="20" spans="2:16">
       <c r="B20" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="E20" s="30" t="s">
         <v>10</v>
@@ -5344,16 +5377,16 @@
         <v>21</v>
       </c>
       <c r="G20" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H20" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K20" s="30" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="L20" s="30" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M20" s="35">
         <v>3.3975</v>
@@ -5370,13 +5403,13 @@
     </row>
     <row r="21" spans="2:16">
       <c r="B21" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="E21" s="31" t="s">
         <v>10</v>
@@ -5385,16 +5418,16 @@
         <v>21</v>
       </c>
       <c r="G21" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K21" s="31" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="L21" s="31" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M21" s="37">
         <v>6.1920000000000002</v>
@@ -5411,13 +5444,13 @@
     </row>
     <row r="22" spans="2:16">
       <c r="B22" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="D22" s="30" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="E22" s="30" t="s">
         <v>10</v>
@@ -5426,39 +5459,39 @@
         <v>21</v>
       </c>
       <c r="G22" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H22" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K22" s="30" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="L22" s="30" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M22" s="35">
-        <v>0.27600000000000002</v>
+        <v>0.89849999999999997</v>
       </c>
       <c r="N22" s="34">
         <v>0.156</v>
       </c>
       <c r="O22" s="32">
-        <v>167.68513401037075</v>
+        <v>164.41834635156846</v>
       </c>
       <c r="P22" s="35">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="2:16">
       <c r="B23" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="E23" s="31" t="s">
         <v>10</v>
@@ -5467,39 +5500,39 @@
         <v>21</v>
       </c>
       <c r="G23" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H23" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K23" s="31" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="L23" s="31" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M23" s="37">
-        <v>0.89849999999999997</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="N23" s="36">
         <v>0.156</v>
       </c>
       <c r="O23" s="33">
-        <v>164.41834635156846</v>
+        <v>167.68513401037075</v>
       </c>
       <c r="P23" s="37">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24" spans="2:16">
       <c r="B24" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="D24" s="30" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="E24" s="30" t="s">
         <v>10</v>
@@ -5508,16 +5541,16 @@
         <v>21</v>
       </c>
       <c r="G24" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H24" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K24" s="30" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="L24" s="30" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M24" s="35">
         <v>4.8682499999999997</v>
@@ -5534,13 +5567,13 @@
     </row>
     <row r="25" spans="2:16">
       <c r="B25" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="E25" s="31" t="s">
         <v>10</v>
@@ -5549,16 +5582,16 @@
         <v>21</v>
       </c>
       <c r="G25" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H25" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K25" s="31" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="L25" s="31" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M25" s="37">
         <v>6.7882499999999997</v>
@@ -5575,13 +5608,13 @@
     </row>
     <row r="26" spans="2:16">
       <c r="B26" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="D26" s="30" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="E26" s="30" t="s">
         <v>10</v>
@@ -5590,16 +5623,16 @@
         <v>21</v>
       </c>
       <c r="G26" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K26" s="30" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="L26" s="30" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M26" s="35">
         <v>1.2615000000000001</v>
@@ -5616,13 +5649,13 @@
     </row>
     <row r="27" spans="2:16">
       <c r="B27" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="D27" s="31" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="E27" s="31" t="s">
         <v>10</v>
@@ -5631,16 +5664,16 @@
         <v>21</v>
       </c>
       <c r="G27" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H27" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K27" s="31" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="L27" s="31" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M27" s="37">
         <v>2.9737499999999999</v>
@@ -5657,13 +5690,13 @@
     </row>
     <row r="28" spans="2:16">
       <c r="B28" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="D28" s="30" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="E28" s="30" t="s">
         <v>10</v>
@@ -5672,16 +5705,16 @@
         <v>21</v>
       </c>
       <c r="G28" s="30" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H28" s="30" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K28" s="30" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="L28" s="30" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M28" s="35">
         <v>0.10725</v>
@@ -5698,13 +5731,13 @@
     </row>
     <row r="29" spans="2:16">
       <c r="B29" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="D29" s="31" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="E29" s="31" t="s">
         <v>10</v>
@@ -5713,16 +5746,16 @@
         <v>21</v>
       </c>
       <c r="G29" s="31" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="H29" s="31" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="K29" s="31" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="L29" s="31" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="M29" s="37">
         <v>0.183</v>
@@ -5747,7 +5780,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20C392E8-42D9-4562-A16F-E389CF5FD676}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B7D8CA1-27C9-4BD2-9BC5-3DCAD7AB24F0}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -5767,7 +5800,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="22.05" customHeight="1">
       <c r="A1" s="27" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B1" s="27"/>
       <c r="C1" s="27"/>
@@ -5779,21 +5812,21 @@
     </row>
     <row r="2" spans="1:17" ht="14.65" thickBot="1">
       <c r="B2" s="28" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="K2" s="28" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="3" spans="1:17" ht="15.75" thickBot="1">
       <c r="B3" s="29" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C3" s="29" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="D3" s="29" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E3" s="29">
         <v>2023</v>
@@ -5805,36 +5838,36 @@
         <v>2050</v>
       </c>
       <c r="H3" s="29" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="K3" s="29" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="L3" s="29" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="M3" s="29" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="N3" s="29" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="O3" s="29" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="P3" s="29" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="Q3" s="29" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
     </row>
     <row r="4" spans="1:17">
       <c r="B4" s="30" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C4" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D4" s="30" t="s">
         <v>19</v>
@@ -5849,13 +5882,13 @@
         <v>0.30000000000000004</v>
       </c>
       <c r="H4" s="30" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="K4" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L4" s="30" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="M4" s="30"/>
       <c r="N4" s="30" t="s">
@@ -5865,18 +5898,18 @@
         <v>21</v>
       </c>
       <c r="P4" s="30" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="Q4" s="30" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="5" spans="1:17">
       <c r="B5" s="31" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D5" s="31" t="s">
         <v>19</v>
@@ -5891,13 +5924,13 @@
         <v>0.60000000000000009</v>
       </c>
       <c r="H5" s="31" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="K5" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L5" s="31" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="M5" s="31"/>
       <c r="N5" s="31" t="s">
@@ -5907,18 +5940,18 @@
         <v>21</v>
       </c>
       <c r="P5" s="31" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="Q5" s="31" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:17">
       <c r="B6" s="30" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C6" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D6" s="30" t="s">
         <v>19</v>
@@ -5933,13 +5966,13 @@
         <v>5100</v>
       </c>
       <c r="H6" s="30" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="K6" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L6" s="30" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="M6" s="30"/>
       <c r="N6" s="30" t="s">
@@ -5949,18 +5982,18 @@
         <v>21</v>
       </c>
       <c r="P6" s="30" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="Q6" s="30" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:17">
       <c r="B7" s="31" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D7" s="31" t="s">
         <v>19</v>
@@ -5975,13 +6008,13 @@
         <v>175</v>
       </c>
       <c r="H7" s="31" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="K7" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L7" s="31" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="M7" s="31"/>
       <c r="N7" s="31" t="s">
@@ -5991,18 +6024,18 @@
         <v>21</v>
       </c>
       <c r="P7" s="31" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="Q7" s="31" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:17">
       <c r="B8" s="30" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="C8" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D8" s="30" t="s">
         <v>19</v>
@@ -6017,13 +6050,13 @@
         <v>3</v>
       </c>
       <c r="H8" s="30" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="K8" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L8" s="30" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="M8" s="30"/>
       <c r="N8" s="30" t="s">
@@ -6033,18 +6066,18 @@
         <v>21</v>
       </c>
       <c r="P8" s="30" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="Q8" s="30" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:17">
       <c r="B9" s="31" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D9" s="31" t="s">
         <v>19</v>
@@ -6059,13 +6092,13 @@
         <v>0.35000000000000003</v>
       </c>
       <c r="H9" s="31" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="K9" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L9" s="31" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="M9" s="31"/>
       <c r="N9" s="31" t="s">
@@ -6075,18 +6108,18 @@
         <v>21</v>
       </c>
       <c r="P9" s="31" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="Q9" s="31" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="10" spans="1:17">
       <c r="B10" s="30" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C10" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D10" s="30" t="s">
         <v>19</v>
@@ -6101,13 +6134,13 @@
         <v>0.60000000000000009</v>
       </c>
       <c r="H10" s="30" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="K10" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L10" s="30" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="M10" s="30"/>
       <c r="N10" s="30" t="s">
@@ -6117,18 +6150,18 @@
         <v>21</v>
       </c>
       <c r="P10" s="30" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="Q10" s="30" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:17">
       <c r="B11" s="31" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C11" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D11" s="31" t="s">
         <v>19</v>
@@ -6143,13 +6176,13 @@
         <v>2300</v>
       </c>
       <c r="H11" s="31" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="K11" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L11" s="31" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="M11" s="31"/>
       <c r="N11" s="31" t="s">
@@ -6159,18 +6192,18 @@
         <v>21</v>
       </c>
       <c r="P11" s="31" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="Q11" s="31" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="12" spans="1:17">
       <c r="B12" s="30" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C12" s="30" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D12" s="30" t="s">
         <v>19</v>
@@ -6185,13 +6218,13 @@
         <v>80</v>
       </c>
       <c r="H12" s="30" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="K12" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L12" s="30" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="M12" s="30"/>
       <c r="N12" s="30" t="s">
@@ -6201,18 +6234,18 @@
         <v>21</v>
       </c>
       <c r="P12" s="30" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="Q12" s="30" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="13" spans="1:17">
       <c r="B13" s="31" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D13" s="31" t="s">
         <v>19</v>
@@ -6227,13 +6260,13 @@
         <v>3</v>
       </c>
       <c r="H13" s="31" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="K13" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L13" s="31" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="M13" s="31"/>
       <c r="N13" s="31" t="s">
@@ -6243,18 +6276,18 @@
         <v>21</v>
       </c>
       <c r="P13" s="31" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="Q13" s="31" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:17">
       <c r="B14" s="30" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D14" s="30" t="s">
         <v>19</v>
@@ -6269,13 +6302,13 @@
         <v>0.61</v>
       </c>
       <c r="H14" s="30" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="K14" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L14" s="30" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="M14" s="30"/>
       <c r="N14" s="30" t="s">
@@ -6285,18 +6318,18 @@
         <v>21</v>
       </c>
       <c r="P14" s="30" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="Q14" s="30" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="15" spans="1:17">
       <c r="B15" s="31" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C15" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D15" s="31" t="s">
         <v>19</v>
@@ -6311,13 +6344,13 @@
         <v>1000</v>
       </c>
       <c r="H15" s="31" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="K15" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L15" s="31" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="M15" s="31"/>
       <c r="N15" s="31" t="s">
@@ -6327,18 +6360,18 @@
         <v>21</v>
       </c>
       <c r="P15" s="31" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="Q15" s="31" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:17">
       <c r="B16" s="30" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C16" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D16" s="30" t="s">
         <v>19</v>
@@ -6353,13 +6386,13 @@
         <v>25</v>
       </c>
       <c r="H16" s="30" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="K16" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L16" s="30" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="M16" s="30"/>
       <c r="N16" s="30" t="s">
@@ -6369,18 +6402,18 @@
         <v>21</v>
       </c>
       <c r="P16" s="30" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="Q16" s="30" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="2:17">
       <c r="B17" s="31" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D17" s="31" t="s">
         <v>19</v>
@@ -6395,13 +6428,13 @@
         <v>0.54</v>
       </c>
       <c r="H17" s="31" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="K17" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L17" s="31" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="M17" s="31"/>
       <c r="N17" s="31" t="s">
@@ -6411,18 +6444,18 @@
         <v>21</v>
       </c>
       <c r="P17" s="31" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="Q17" s="31" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="18" spans="2:17">
       <c r="B18" s="30" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C18" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="30" t="s">
         <v>19</v>
@@ -6437,13 +6470,13 @@
         <v>2400</v>
       </c>
       <c r="H18" s="30" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="K18" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L18" s="30" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="M18" s="30"/>
       <c r="N18" s="30" t="s">
@@ -6453,18 +6486,18 @@
         <v>21</v>
       </c>
       <c r="P18" s="30" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="Q18" s="30" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="2:17">
       <c r="B19" s="31" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="C19" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D19" s="31" t="s">
         <v>19</v>
@@ -6479,13 +6512,13 @@
         <v>60</v>
       </c>
       <c r="H19" s="31" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="K19" s="31" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L19" s="31" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="M19" s="31"/>
       <c r="N19" s="31" t="s">
@@ -6495,18 +6528,18 @@
         <v>21</v>
       </c>
       <c r="P19" s="31" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="Q19" s="31" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="20" spans="2:17">
       <c r="B20" s="30" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D20" s="30" t="s">
         <v>19</v>
@@ -6521,13 +6554,13 @@
         <v>0.39</v>
       </c>
       <c r="H20" s="30" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="K20" s="30" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="L20" s="30" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="M20" s="30"/>
       <c r="N20" s="30" t="s">
@@ -6537,18 +6570,18 @@
         <v>21</v>
       </c>
       <c r="P20" s="30" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="Q20" s="30" t="s">
-        <v>243</v>
+        <v>246</v>
       </c>
     </row>
     <row r="21" spans="2:17">
       <c r="B21" s="31" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C21" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D21" s="31" t="s">
         <v>19</v>
@@ -6563,15 +6596,15 @@
         <v>4350</v>
       </c>
       <c r="H21" s="31" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="2:17">
       <c r="B22" s="30" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D22" s="30" t="s">
         <v>19</v>
@@ -6586,15 +6619,15 @@
         <v>130</v>
       </c>
       <c r="H22" s="30" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="23" spans="2:17">
       <c r="B23" s="31" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D23" s="31" t="s">
         <v>19</v>
@@ -6609,15 +6642,15 @@
         <v>0.42</v>
       </c>
       <c r="H23" s="31" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="24" spans="2:17">
       <c r="B24" s="30" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C24" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D24" s="30" t="s">
         <v>19</v>
@@ -6632,15 +6665,15 @@
         <v>500</v>
       </c>
       <c r="H24" s="30" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="2:17">
       <c r="B25" s="31" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="C25" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D25" s="31" t="s">
         <v>19</v>
@@ -6655,15 +6688,15 @@
         <v>20</v>
       </c>
       <c r="H25" s="31" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="26" spans="2:17">
       <c r="B26" s="30" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C26" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" s="30" t="s">
         <v>19</v>
@@ -6678,15 +6711,15 @@
         <v>1</v>
       </c>
       <c r="H26" s="30" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="27" spans="2:17">
       <c r="B27" s="31" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C27" s="31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D27" s="31" t="s">
         <v>19</v>
@@ -6701,15 +6734,15 @@
         <v>0.35000000000000003</v>
       </c>
       <c r="H27" s="31" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="28" spans="2:17">
       <c r="B28" s="30" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C28" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D28" s="30" t="s">
         <v>19</v>
@@ -6724,15 +6757,15 @@
         <v>2650</v>
       </c>
       <c r="H28" s="30" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="29" spans="2:17">
       <c r="B29" s="31" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C29" s="31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D29" s="31" t="s">
         <v>19</v>
@@ -6747,15 +6780,15 @@
         <v>65</v>
       </c>
       <c r="H29" s="31" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="30" spans="2:17">
       <c r="B30" s="30" t="s">
-        <v>231</v>
+        <v>234</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D30" s="30" t="s">
         <v>19</v>
@@ -6770,15 +6803,15 @@
         <v>4</v>
       </c>
       <c r="H30" s="30" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="31" spans="2:17">
       <c r="B31" s="31" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C31" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D31" s="31" t="s">
         <v>19</v>
@@ -6793,15 +6826,15 @@
         <v>0.5</v>
       </c>
       <c r="H31" s="31" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="32" spans="2:17">
       <c r="B32" s="30" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C32" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D32" s="30" t="s">
         <v>19</v>
@@ -6816,15 +6849,15 @@
         <v>2300</v>
       </c>
       <c r="H32" s="30" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="33" spans="2:8">
       <c r="B33" s="31" t="s">
-        <v>232</v>
+        <v>235</v>
       </c>
       <c r="C33" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D33" s="31" t="s">
         <v>19</v>
@@ -6839,15 +6872,15 @@
         <v>80</v>
       </c>
       <c r="H33" s="31" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="2:8">
       <c r="B34" s="30" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C34" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D34" s="30" t="s">
         <v>19</v>
@@ -6862,15 +6895,15 @@
         <v>0.43</v>
       </c>
       <c r="H34" s="30" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="35" spans="2:8">
       <c r="B35" s="31" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C35" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D35" s="31" t="s">
         <v>19</v>
@@ -6885,15 +6918,15 @@
         <v>5100</v>
       </c>
       <c r="H35" s="31" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="36" spans="2:8">
       <c r="B36" s="30" t="s">
-        <v>233</v>
+        <v>236</v>
       </c>
       <c r="C36" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D36" s="30" t="s">
         <v>19</v>
@@ -6908,15 +6941,15 @@
         <v>180</v>
       </c>
       <c r="H36" s="30" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="37" spans="2:8">
       <c r="B37" s="31" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C37" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D37" s="31" t="s">
         <v>19</v>
@@ -6931,15 +6964,15 @@
         <v>0.33</v>
       </c>
       <c r="H37" s="31" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="38" spans="2:8">
       <c r="B38" s="30" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C38" s="30" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D38" s="30" t="s">
         <v>19</v>
@@ -6954,15 +6987,15 @@
         <v>4500</v>
       </c>
       <c r="H38" s="30" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="39" spans="2:8">
       <c r="B39" s="31" t="s">
-        <v>234</v>
+        <v>237</v>
       </c>
       <c r="C39" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D39" s="31" t="s">
         <v>19</v>
@@ -6977,15 +7010,15 @@
         <v>160</v>
       </c>
       <c r="H39" s="31" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="40" spans="2:8">
       <c r="B40" s="30" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C40" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D40" s="30" t="s">
         <v>19</v>
@@ -7000,15 +7033,15 @@
         <v>0.39</v>
       </c>
       <c r="H40" s="30" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="41" spans="2:8">
       <c r="B41" s="31" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C41" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D41" s="31" t="s">
         <v>19</v>
@@ -7023,15 +7056,15 @@
         <v>5100</v>
       </c>
       <c r="H41" s="31" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="42" spans="2:8">
       <c r="B42" s="30" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="C42" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D42" s="30" t="s">
         <v>19</v>
@@ -7046,15 +7079,15 @@
         <v>155</v>
       </c>
       <c r="H42" s="30" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43" spans="2:8">
       <c r="B43" s="31" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D43" s="31" t="s">
         <v>19</v>
@@ -7069,15 +7102,15 @@
         <v>1</v>
       </c>
       <c r="H43" s="31" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="44" spans="2:8">
       <c r="B44" s="30" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C44" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D44" s="30" t="s">
         <v>19</v>
@@ -7092,15 +7125,15 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="H44" s="30" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="2:8">
       <c r="B45" s="31" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C45" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D45" s="31" t="s">
         <v>19</v>
@@ -7115,15 +7148,15 @@
         <v>340</v>
       </c>
       <c r="H45" s="31" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="46" spans="2:8">
       <c r="B46" s="30" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C46" s="30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D46" s="30" t="s">
         <v>19</v>
@@ -7138,15 +7171,15 @@
         <v>10</v>
       </c>
       <c r="H46" s="30" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="47" spans="2:8">
       <c r="B47" s="31" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="C47" s="31" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D47" s="31" t="s">
         <v>19</v>
@@ -7161,15 +7194,15 @@
         <v>1.5</v>
       </c>
       <c r="H47" s="31" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="48" spans="2:8">
       <c r="B48" s="30" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C48" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D48" s="30" t="s">
         <v>19</v>
@@ -7184,15 +7217,15 @@
         <v>0.39</v>
       </c>
       <c r="H48" s="30" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="49" spans="2:8">
       <c r="B49" s="31" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C49" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D49" s="31" t="s">
         <v>19</v>
@@ -7207,15 +7240,15 @@
         <v>1700</v>
       </c>
       <c r="H49" s="31" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="50" spans="2:8">
       <c r="B50" s="30" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="C50" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D50" s="30" t="s">
         <v>19</v>
@@ -7230,15 +7263,15 @@
         <v>45</v>
       </c>
       <c r="H50" s="30" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="51" spans="2:8">
       <c r="B51" s="31" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C51" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D51" s="31" t="s">
         <v>19</v>
@@ -7253,15 +7286,15 @@
         <v>0.43</v>
       </c>
       <c r="H51" s="31" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="52" spans="2:8">
       <c r="B52" s="30" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C52" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D52" s="30" t="s">
         <v>19</v>
@@ -7276,15 +7309,15 @@
         <v>2000</v>
       </c>
       <c r="H52" s="30" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="53" spans="2:8">
       <c r="B53" s="31" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="C53" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D53" s="31" t="s">
         <v>19</v>
@@ -7299,15 +7332,15 @@
         <v>60</v>
       </c>
       <c r="H53" s="31" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="54" spans="2:8">
       <c r="B54" s="30" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C54" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D54" s="30" t="s">
         <v>19</v>
@@ -7322,15 +7355,15 @@
         <v>0.48</v>
       </c>
       <c r="H54" s="30" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="55" spans="2:8">
       <c r="B55" s="31" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C55" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D55" s="31" t="s">
         <v>19</v>
@@ -7345,15 +7378,15 @@
         <v>2200</v>
       </c>
       <c r="H55" s="31" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="56" spans="2:8">
       <c r="B56" s="30" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="C56" s="30" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D56" s="30" t="s">
         <v>19</v>
@@ -7368,15 +7401,15 @@
         <v>65</v>
       </c>
       <c r="H56" s="30" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="57" spans="2:8">
       <c r="B57" s="31" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D57" s="31" t="s">
         <v>19</v>
@@ -7391,15 +7424,15 @@
         <v>1</v>
       </c>
       <c r="H57" s="31" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="58" spans="2:8">
       <c r="B58" s="30" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C58" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D58" s="30" t="s">
         <v>19</v>
@@ -7414,15 +7447,15 @@
         <v>0.56000000000000005</v>
       </c>
       <c r="H58" s="30" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="59" spans="2:8">
       <c r="B59" s="31" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D59" s="31" t="s">
         <v>19</v>
@@ -7437,15 +7470,15 @@
         <v>1660</v>
       </c>
       <c r="H59" s="31" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="60" spans="2:8">
       <c r="B60" s="30" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C60" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D60" s="30" t="s">
         <v>19</v>
@@ -7460,15 +7493,15 @@
         <v>40</v>
       </c>
       <c r="H60" s="30" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="61" spans="2:8">
       <c r="B61" s="31" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="C61" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D61" s="31" t="s">
         <v>19</v>
@@ -7483,15 +7516,15 @@
         <v>3</v>
       </c>
       <c r="H61" s="31" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
     <row r="62" spans="2:8">
       <c r="B62" s="30" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C62" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D62" s="30" t="s">
         <v>19</v>
@@ -7506,15 +7539,15 @@
         <v>1</v>
       </c>
       <c r="H62" s="30" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
     </row>
     <row r="63" spans="2:8">
       <c r="B63" s="31" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C63" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D63" s="31" t="s">
         <v>19</v>
@@ -7529,15 +7562,15 @@
         <v>0.3</v>
       </c>
       <c r="H63" s="31" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
     </row>
     <row r="64" spans="2:8">
       <c r="B64" s="30" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C64" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D64" s="30" t="s">
         <v>19</v>
@@ -7552,15 +7585,15 @@
         <v>1490</v>
       </c>
       <c r="H64" s="30" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
     </row>
     <row r="65" spans="2:8">
       <c r="B65" s="31" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C65" s="31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D65" s="31" t="s">
         <v>19</v>
@@ -7575,15 +7608,15 @@
         <v>38</v>
       </c>
       <c r="H65" s="31" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
     </row>
     <row r="66" spans="2:8">
       <c r="B66" s="30" t="s">
-        <v>241</v>
+        <v>244</v>
       </c>
       <c r="C66" s="30" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D66" s="30" t="s">
         <v>19</v>
@@ -7598,7 +7631,7 @@
         <v>1.5</v>
       </c>
       <c r="H66" s="30" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated CHE model - 2025-08-17 01:15
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{398E2FA7-BE01-4237-A61D-02DD81742470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E258BE2-E1B6-4196-B3B3-15A4D5D0EFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3675" yWindow="3675" windowWidth="21600" windowHeight="12683" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="misc" sheetId="7" r:id="rId1"/>
@@ -668,16 +668,16 @@
     <t>wind resource -- CF class won-CHE_22 -- cost class 3</t>
   </si>
   <si>
+    <t>e_won-CHE_20_c1</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-CHE_20 -- cost class 1</t>
+  </si>
+  <si>
     <t>e_won-CHE_20_c2</t>
   </si>
   <si>
     <t>wind resource -- CF class won-CHE_20 -- cost class 2</t>
-  </si>
-  <si>
-    <t>e_won-CHE_20_c1</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-CHE_20 -- cost class 1</t>
   </si>
   <si>
     <t>e_won-CHE_18_c2</t>
@@ -1221,7 +1221,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F57F225B-449B-0A31-AAEF-5355EEE29B47}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8337E6BC-7249-F19E-5FBA-545596705A4E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1276,7 +1276,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6998E14A-D71B-790A-D7D3-7B3AFAE2D8E6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B0BA174-4BBC-217F-5D6E-D5BF30705C07}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1331,7 +1331,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44B01E60-5C1C-919C-C440-D6926EAC786E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{798A8E3D-3362-EA88-3C92-FEE96287A30B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1386,7 +1386,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E34A19BF-D748-BCD1-BF0F-423BD8E750FC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B82A2D10-1E3A-11CE-6331-5682F0CDF286}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3913,7 +3913,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4186DA58-E7A0-4982-96AF-F2941C12B474}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{420361EE-111E-4C9F-99D9-2E9F053DACBD}">
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4621,7 +4621,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E354DA90-C15C-4AB0-B806-99F5508204B4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6BDA2AD-FDD0-478D-85BA-F0A7B09FD489}">
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5102,16 +5102,16 @@
         <v>221</v>
       </c>
       <c r="M13" s="37">
-        <v>0.30525000000000002</v>
+        <v>4.6582499999999998</v>
       </c>
       <c r="N13" s="36">
         <v>0.19600000000000001</v>
       </c>
       <c r="O13" s="33">
-        <v>170.53727340823224</v>
+        <v>91.771393190446332</v>
       </c>
       <c r="P13" s="37">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -5143,16 +5143,16 @@
         <v>221</v>
       </c>
       <c r="M14" s="35">
-        <v>4.6582499999999998</v>
+        <v>0.30525000000000002</v>
       </c>
       <c r="N14" s="34">
         <v>0.19600000000000001</v>
       </c>
       <c r="O14" s="32">
-        <v>91.771393190446332</v>
+        <v>170.53727340823224</v>
       </c>
       <c r="P14" s="35">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -5780,7 +5780,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B7D8CA1-27C9-4BD2-9BC5-3DCAD7AB24F0}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC007E0-ED18-4603-9E9D-D123D368A352}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE model - 2025-08-17 01:37
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E258BE2-E1B6-4196-B3B3-15A4D5D0EFF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B39F88E-EE88-4B04-8256-B2C49A8FE59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3675" yWindow="3675" windowWidth="21600" windowHeight="12683" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2573" yWindow="2573" windowWidth="21600" windowHeight="12682" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="misc" sheetId="7" r:id="rId1"/>
@@ -500,24 +500,24 @@
     <t>ele</t>
   </si>
   <si>
+    <t>e_spv-CHE_15_c2</t>
+  </si>
+  <si>
+    <t>solar resource -- CF class spv-CHE_15 -- cost class 2</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
     <t>e_spv-CHE_15_c3</t>
   </si>
   <si>
     <t>solar resource -- CF class spv-CHE_15 -- cost class 3</t>
   </si>
   <si>
-    <t>annual</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>e_spv-CHE_15_c2</t>
-  </si>
-  <si>
-    <t>solar resource -- CF class spv-CHE_15 -- cost class 2</t>
-  </si>
-  <si>
     <t>e_spv-CHE_15_c1</t>
   </si>
   <si>
@@ -668,18 +668,18 @@
     <t>wind resource -- CF class won-CHE_22 -- cost class 3</t>
   </si>
   <si>
+    <t>e_won-CHE_20_c2</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-CHE_20 -- cost class 2</t>
+  </si>
+  <si>
     <t>e_won-CHE_20_c1</t>
   </si>
   <si>
     <t>wind resource -- CF class won-CHE_20 -- cost class 1</t>
   </si>
   <si>
-    <t>e_won-CHE_20_c2</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-CHE_20 -- cost class 2</t>
-  </si>
-  <si>
     <t>e_won-CHE_18_c2</t>
   </si>
   <si>
@@ -722,28 +722,28 @@
     <t>wind resource -- CF class won-CHE_16 -- cost class 1</t>
   </si>
   <si>
+    <t>e_won-CHE_16_c3</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-CHE_16 -- cost class 3</t>
+  </si>
+  <si>
     <t>e_won-CHE_16_c2</t>
   </si>
   <si>
     <t>wind resource -- CF class won-CHE_16 -- cost class 2</t>
   </si>
   <si>
-    <t>e_won-CHE_16_c3</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-CHE_16 -- cost class 3</t>
+    <t>e_won-CHE_15_c2</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-CHE_15 -- cost class 2</t>
   </si>
   <si>
     <t>e_won-CHE_15_c1</t>
   </si>
   <si>
     <t>wind resource -- CF class won-CHE_15 -- cost class 1</t>
-  </si>
-  <si>
-    <t>e_won-CHE_15_c2</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-CHE_15 -- cost class 2</t>
   </si>
   <si>
     <t>e_won-CHE_14_c3</t>
@@ -1221,7 +1221,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8337E6BC-7249-F19E-5FBA-545596705A4E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EC01191-B265-0251-BF8B-3E3C9EDCF037}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1276,7 +1276,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B0BA174-4BBC-217F-5D6E-D5BF30705C07}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C84BE452-A200-2591-844A-561362373AFB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1331,7 +1331,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{798A8E3D-3362-EA88-3C92-FEE96287A30B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{886F61FA-918A-72CE-6B40-9A1D7151B578}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1386,7 +1386,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B82A2D10-1E3A-11CE-6331-5682F0CDF286}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38A85FF9-9585-A6C5-732C-4B6D350C9856}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3913,7 +3913,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{420361EE-111E-4C9F-99D9-2E9F053DACBD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E228FF-4B9C-49FB-A02B-AF26906E2F0D}">
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4025,16 +4025,16 @@
         <v>168</v>
       </c>
       <c r="M4" s="34">
-        <v>6.7499999999999999E-3</v>
+        <v>4.725E-2</v>
       </c>
       <c r="N4" s="34">
         <v>0.14799999999999999</v>
       </c>
       <c r="O4" s="32">
-        <v>58.670132479893049</v>
+        <v>57.399715057025539</v>
       </c>
       <c r="P4" s="35">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -4066,16 +4066,16 @@
         <v>168</v>
       </c>
       <c r="M5" s="36">
-        <v>4.725E-2</v>
+        <v>6.7499999999999999E-3</v>
       </c>
       <c r="N5" s="36">
         <v>0.14799999999999999</v>
       </c>
       <c r="O5" s="33">
-        <v>57.399715057025539</v>
+        <v>58.670132479893049</v>
       </c>
       <c r="P5" s="37">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -4621,7 +4621,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6BDA2AD-FDD0-478D-85BA-F0A7B09FD489}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C02F3C1-1B03-4404-B101-C0C5F392FB75}">
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5102,16 +5102,16 @@
         <v>221</v>
       </c>
       <c r="M13" s="37">
-        <v>4.6582499999999998</v>
+        <v>0.30525000000000002</v>
       </c>
       <c r="N13" s="36">
         <v>0.19600000000000001</v>
       </c>
       <c r="O13" s="33">
-        <v>91.771393190446332</v>
+        <v>170.53727340823224</v>
       </c>
       <c r="P13" s="37">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -5143,16 +5143,16 @@
         <v>221</v>
       </c>
       <c r="M14" s="35">
-        <v>0.30525000000000002</v>
+        <v>4.6582499999999998</v>
       </c>
       <c r="N14" s="34">
         <v>0.19600000000000001</v>
       </c>
       <c r="O14" s="32">
-        <v>170.53727340823224</v>
+        <v>91.771393190446332</v>
       </c>
       <c r="P14" s="35">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -5471,16 +5471,16 @@
         <v>221</v>
       </c>
       <c r="M22" s="35">
-        <v>0.89849999999999997</v>
+        <v>0.27600000000000002</v>
       </c>
       <c r="N22" s="34">
         <v>0.156</v>
       </c>
       <c r="O22" s="32">
-        <v>164.41834635156846</v>
+        <v>167.68513401037075</v>
       </c>
       <c r="P22" s="35">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="23" spans="2:16">
@@ -5512,16 +5512,16 @@
         <v>221</v>
       </c>
       <c r="M23" s="37">
-        <v>0.27600000000000002</v>
+        <v>0.89849999999999997</v>
       </c>
       <c r="N23" s="36">
         <v>0.156</v>
       </c>
       <c r="O23" s="33">
-        <v>167.68513401037075</v>
+        <v>164.41834635156846</v>
       </c>
       <c r="P23" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="2:16">
@@ -5553,16 +5553,16 @@
         <v>221</v>
       </c>
       <c r="M24" s="35">
-        <v>4.8682499999999997</v>
+        <v>6.7882499999999997</v>
       </c>
       <c r="N24" s="34">
         <v>0.153</v>
       </c>
       <c r="O24" s="32">
-        <v>84.517079807307184</v>
+        <v>99.126880170283727</v>
       </c>
       <c r="P24" s="35">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="2:16">
@@ -5594,16 +5594,16 @@
         <v>221</v>
       </c>
       <c r="M25" s="37">
-        <v>6.7882499999999997</v>
+        <v>4.8682499999999997</v>
       </c>
       <c r="N25" s="36">
         <v>0.153</v>
       </c>
       <c r="O25" s="33">
-        <v>99.126880170283727</v>
+        <v>84.517079807307184</v>
       </c>
       <c r="P25" s="37">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="2:16">
@@ -5780,7 +5780,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CC007E0-ED18-4603-9E9D-D123D368A352}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A270ADD-F877-4297-877A-2DDBECE0B792}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE model - 2025-08-17 15:03
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5B39F88E-EE88-4B04-8256-B2C49A8FE59F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFC93723-3857-4D22-80A3-1020BA1979EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2573" yWindow="2573" windowWidth="21600" windowHeight="12682" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="misc" sheetId="7" r:id="rId1"/>
@@ -500,24 +500,24 @@
     <t>ele</t>
   </si>
   <si>
+    <t>e_spv-CHE_15_c3</t>
+  </si>
+  <si>
+    <t>solar resource -- CF class spv-CHE_15 -- cost class 3</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
     <t>e_spv-CHE_15_c2</t>
   </si>
   <si>
     <t>solar resource -- CF class spv-CHE_15 -- cost class 2</t>
   </si>
   <si>
-    <t>annual</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>e_spv-CHE_15_c3</t>
-  </si>
-  <si>
-    <t>solar resource -- CF class spv-CHE_15 -- cost class 3</t>
-  </si>
-  <si>
     <t>e_spv-CHE_15_c1</t>
   </si>
   <si>
@@ -668,18 +668,18 @@
     <t>wind resource -- CF class won-CHE_22 -- cost class 3</t>
   </si>
   <si>
+    <t>e_won-CHE_20_c1</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-CHE_20 -- cost class 1</t>
+  </si>
+  <si>
     <t>e_won-CHE_20_c2</t>
   </si>
   <si>
     <t>wind resource -- CF class won-CHE_20 -- cost class 2</t>
   </si>
   <si>
-    <t>e_won-CHE_20_c1</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-CHE_20 -- cost class 1</t>
-  </si>
-  <si>
     <t>e_won-CHE_18_c2</t>
   </si>
   <si>
@@ -734,16 +734,16 @@
     <t>wind resource -- CF class won-CHE_16 -- cost class 2</t>
   </si>
   <si>
+    <t>e_won-CHE_15_c1</t>
+  </si>
+  <si>
+    <t>wind resource -- CF class won-CHE_15 -- cost class 1</t>
+  </si>
+  <si>
     <t>e_won-CHE_15_c2</t>
   </si>
   <si>
     <t>wind resource -- CF class won-CHE_15 -- cost class 2</t>
-  </si>
-  <si>
-    <t>e_won-CHE_15_c1</t>
-  </si>
-  <si>
-    <t>wind resource -- CF class won-CHE_15 -- cost class 1</t>
   </si>
   <si>
     <t>e_won-CHE_14_c3</t>
@@ -1221,7 +1221,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0EC01191-B265-0251-BF8B-3E3C9EDCF037}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADF7671D-55EA-850D-C603-A334D2415965}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1276,7 +1276,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C84BE452-A200-2591-844A-561362373AFB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCD654A7-FF6A-4059-1E8C-427C1C204040}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1331,7 +1331,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{886F61FA-918A-72CE-6B40-9A1D7151B578}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44F36A59-6BE3-3B1C-0B83-E9240EA3C9A0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1386,7 +1386,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{38A85FF9-9585-A6C5-732C-4B6D350C9856}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB5AA6ED-0260-4EBF-924A-59A43584E271}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3913,7 +3913,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13E228FF-4B9C-49FB-A02B-AF26906E2F0D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF955AFC-B9B5-4779-9C14-2980258AC0F1}">
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4025,16 +4025,16 @@
         <v>168</v>
       </c>
       <c r="M4" s="34">
-        <v>4.725E-2</v>
+        <v>6.7499999999999999E-3</v>
       </c>
       <c r="N4" s="34">
         <v>0.14799999999999999</v>
       </c>
       <c r="O4" s="32">
-        <v>57.399715057025539</v>
+        <v>58.670132479893049</v>
       </c>
       <c r="P4" s="35">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -4066,16 +4066,16 @@
         <v>168</v>
       </c>
       <c r="M5" s="36">
-        <v>6.7499999999999999E-3</v>
+        <v>4.725E-2</v>
       </c>
       <c r="N5" s="36">
         <v>0.14799999999999999</v>
       </c>
       <c r="O5" s="33">
-        <v>58.670132479893049</v>
+        <v>57.399715057025539</v>
       </c>
       <c r="P5" s="37">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -4621,7 +4621,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C02F3C1-1B03-4404-B101-C0C5F392FB75}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB854EBE-2F8E-4326-ADB4-8CA4D056EDCF}">
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5102,16 +5102,16 @@
         <v>221</v>
       </c>
       <c r="M13" s="37">
-        <v>0.30525000000000002</v>
+        <v>4.6582499999999998</v>
       </c>
       <c r="N13" s="36">
         <v>0.19600000000000001</v>
       </c>
       <c r="O13" s="33">
-        <v>170.53727340823224</v>
+        <v>91.771393190446332</v>
       </c>
       <c r="P13" s="37">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:16">
@@ -5143,16 +5143,16 @@
         <v>221</v>
       </c>
       <c r="M14" s="35">
-        <v>4.6582499999999998</v>
+        <v>0.30525000000000002</v>
       </c>
       <c r="N14" s="34">
         <v>0.19600000000000001</v>
       </c>
       <c r="O14" s="32">
-        <v>91.771393190446332</v>
+        <v>170.53727340823224</v>
       </c>
       <c r="P14" s="35">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:16">
@@ -5553,16 +5553,16 @@
         <v>221</v>
       </c>
       <c r="M24" s="35">
-        <v>6.7882499999999997</v>
+        <v>4.8682499999999997</v>
       </c>
       <c r="N24" s="34">
         <v>0.153</v>
       </c>
       <c r="O24" s="32">
-        <v>99.126880170283727</v>
+        <v>84.517079807307184</v>
       </c>
       <c r="P24" s="35">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="2:16">
@@ -5594,16 +5594,16 @@
         <v>221</v>
       </c>
       <c r="M25" s="37">
-        <v>4.8682499999999997</v>
+        <v>6.7882499999999997</v>
       </c>
       <c r="N25" s="36">
         <v>0.153</v>
       </c>
       <c r="O25" s="33">
-        <v>84.517079807307184</v>
+        <v>99.126880170283727</v>
       </c>
       <c r="P25" s="37">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="26" spans="2:16">
@@ -5780,7 +5780,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A270ADD-F877-4297-877A-2DDBECE0B792}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABC3172-E736-43B9-950E-A425E7092401}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE model - 2025-08-17 21:33
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFC93723-3857-4D22-80A3-1020BA1979EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5D8F7956-5DCF-45BA-8672-D3EBEA1B46F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="6" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -500,22 +500,22 @@
     <t>ele</t>
   </si>
   <si>
+    <t>e_spv-CHE_15_c2</t>
+  </si>
+  <si>
+    <t>solar resource -- CF class spv-CHE_15 -- cost class 2</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
     <t>e_spv-CHE_15_c3</t>
   </si>
   <si>
     <t>solar resource -- CF class spv-CHE_15 -- cost class 3</t>
-  </si>
-  <si>
-    <t>annual</t>
-  </si>
-  <si>
-    <t>no</t>
-  </si>
-  <si>
-    <t>e_spv-CHE_15_c2</t>
-  </si>
-  <si>
-    <t>solar resource -- CF class spv-CHE_15 -- cost class 2</t>
   </si>
   <si>
     <t>e_spv-CHE_15_c1</t>
@@ -1221,7 +1221,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ADF7671D-55EA-850D-C603-A334D2415965}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2A0987BF-A5B9-48CF-76E5-B439790A7AD0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1276,7 +1276,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BCD654A7-FF6A-4059-1E8C-427C1C204040}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6F8E22A-BDCE-4260-E169-10AAEDC2BE81}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1331,7 +1331,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{44F36A59-6BE3-3B1C-0B83-E9240EA3C9A0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0A5CE3BF-0DB3-78FF-BD81-59BEF365F370}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1386,7 +1386,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EB5AA6ED-0260-4EBF-924A-59A43584E271}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9305617-D47D-E29D-3A48-4997C6419789}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3913,7 +3913,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF955AFC-B9B5-4779-9C14-2980258AC0F1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4497D131-825D-486D-B66F-8CAC64302E5F}">
   <dimension ref="A1:P18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4025,16 +4025,16 @@
         <v>168</v>
       </c>
       <c r="M4" s="34">
-        <v>6.7499999999999999E-3</v>
+        <v>4.725E-2</v>
       </c>
       <c r="N4" s="34">
         <v>0.14799999999999999</v>
       </c>
       <c r="O4" s="32">
-        <v>58.670132479893049</v>
+        <v>57.399715057025539</v>
       </c>
       <c r="P4" s="35">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:16">
@@ -4066,16 +4066,16 @@
         <v>168</v>
       </c>
       <c r="M5" s="36">
-        <v>4.725E-2</v>
+        <v>6.7499999999999999E-3</v>
       </c>
       <c r="N5" s="36">
         <v>0.14799999999999999</v>
       </c>
       <c r="O5" s="33">
-        <v>57.399715057025539</v>
+        <v>58.670132479893049</v>
       </c>
       <c r="P5" s="37">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:16">
@@ -4621,7 +4621,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB854EBE-2F8E-4326-ADB4-8CA4D056EDCF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B91FF6F-FB00-46F8-BD8A-EC7FDE49122E}">
   <dimension ref="A1:P29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5780,7 +5780,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ABC3172-E736-43B9-950E-A425E7092401}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B143CA6-6B8A-4BB8-AB3B-911B7DE0D82C}">
   <dimension ref="A1:Q66"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE model - 2025-09-06 17:22
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07C7C1A6-DDE7-4201-B4E2-FEBD1143E4A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B61F2A0-0183-417C-BE65-646FA70FDB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5910,7 +5910,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE278324-E0C0-4271-815F-C1CA19F06B12}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34DFEC0-B882-4A80-A073-B1AA0C7037BF}">
   <dimension ref="B9:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6767,7 +6767,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDD5CE1A-86C1-4D45-92DB-AF8660955D68}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A06E4CC-07B9-4E94-B6EC-69FEB032B706}">
   <dimension ref="B9:AB31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7666,7 +7666,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE4B4277-11DF-48E4-88AC-15FE33A582EC}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A40DACA-A9E3-4D7D-8705-505213D63C19}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE model - 2025-09-06 20:15
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B61F2A0-0183-417C-BE65-646FA70FDB35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{340EAAE5-3D89-4E88-AE7B-AEB43DAF5B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5910,7 +5910,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C34DFEC0-B882-4A80-A073-B1AA0C7037BF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA1A250-B7D5-4641-B248-767527D3B1A1}">
   <dimension ref="B9:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6767,7 +6767,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A06E4CC-07B9-4E94-B6EC-69FEB032B706}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A07297B-08CB-466D-9096-A2E9F076C89C}">
   <dimension ref="B9:AB31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7666,7 +7666,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5A40DACA-A9E3-4D7D-8705-505213D63C19}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C3FDF01-B7C7-4E49-BF36-EBE0D2917A22}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE model - 2025-09-06 20:19
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{340EAAE5-3D89-4E88-AE7B-AEB43DAF5B58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{03EE48B9-6BD9-4465-9976-FCCA7F0C9C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5910,7 +5910,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DAA1A250-B7D5-4641-B248-767527D3B1A1}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136828E3-CC66-4AD5-A2C8-ABA62CEED807}">
   <dimension ref="B9:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6767,7 +6767,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A07297B-08CB-466D-9096-A2E9F076C89C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70FC6E2-0A39-4A16-B80E-EF4415E55F67}">
   <dimension ref="B9:AB31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7666,7 +7666,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C3FDF01-B7C7-4E49-BF36-EBE0D2917A22}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{214BE021-8116-4CD8-A84C-5B107B3050EE}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE model - 2025-09-06 20:23
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{03EE48B9-6BD9-4465-9976-FCCA7F0C9C62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FE38DAB-8601-42E7-A8A4-9F911B997DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5910,7 +5910,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{136828E3-CC66-4AD5-A2C8-ABA62CEED807}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72BD7EFD-9FC8-4537-9E90-C830EEC50B95}">
   <dimension ref="B9:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6767,7 +6767,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C70FC6E2-0A39-4A16-B80E-EF4415E55F67}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD93065D-8024-4C6E-A1FF-E13C9817E6C2}">
   <dimension ref="B9:AB31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7666,7 +7666,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{214BE021-8116-4CD8-A84C-5B107B3050EE}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB42B990-6F3C-4E2B-BD51-8C821F0BAD0F}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>

<commit_message>
Updated CHE model - 2025-09-06 20:30
</commit_message>
<xml_diff>
--- a/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
+++ b/VerveStacks_CHE/SubRES_Tmpl/SubRES_New_RE_and_Conventional.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_CHE\SubRES_Tmpl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5FE38DAB-8601-42E7-A8A4-9F911B997DA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{634C8EDC-DE9A-455A-A530-036AE25895D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" firstSheet="7" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5910,7 +5910,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72BD7EFD-9FC8-4537-9E90-C830EEC50B95}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3FA35B1-6A29-4AD0-96CE-9B08AFFF93CA}">
   <dimension ref="B9:N31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -6767,7 +6767,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD93065D-8024-4C6E-A1FF-E13C9817E6C2}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2218FD5-92EB-450B-B5EE-1FC0BC5D2E1B}">
   <dimension ref="B9:AB31"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -7666,7 +7666,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB42B990-6F3C-4E2B-BD51-8C821F0BAD0F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{758EE043-ADCC-44DF-938E-E08DA8D03D96}">
   <dimension ref="B9:P73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>